<commit_message>
adding a temp row to s_other
</commit_message>
<xml_diff>
--- a/input/settings/s_other.xlsx
+++ b/input/settings/s_other.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuzzy\BKsDBTools\summoners_war_0_1_0\input\settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuzzy\bk_sw_tools_DEV\input\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="7800" windowHeight="3870"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="7800" windowHeight="3870"/>
   </bookViews>
   <sheets>
     <sheet name="s_player_unit" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
   <si>
     <t>unit_id</t>
   </si>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t>World Arena, Real-Time Arena</t>
+  </si>
+  <si>
+    <t>Lapis (Water Magic Knight)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Lapis (Water Magic Knight) lvl 40 | 999999</t>
   </si>
 </sst>
 </file>
@@ -444,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -470,11 +482,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -488,6 +531,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,66 +974,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV1"/>
+  <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="24.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="62.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="62.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1127,6 +1177,150 @@
       </c>
       <c r="AV1" s="10" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>999999</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="11">
+        <v>40</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1</v>
+      </c>
+      <c r="J2" s="11">
+        <v>1</v>
+      </c>
+      <c r="K2" s="11">
+        <v>1</v>
+      </c>
+      <c r="L2" s="11">
+        <v>1</v>
+      </c>
+      <c r="M2" s="11">
+        <v>1</v>
+      </c>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="P2" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>1</v>
+      </c>
+      <c r="R2" s="11">
+        <v>1</v>
+      </c>
+      <c r="S2" s="11">
+        <v>1</v>
+      </c>
+      <c r="T2" s="11">
+        <v>1</v>
+      </c>
+      <c r="U2" s="11">
+        <v>1</v>
+      </c>
+      <c r="V2" s="11">
+        <v>1</v>
+      </c>
+      <c r="W2" s="11">
+        <v>1</v>
+      </c>
+      <c r="X2" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="11">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AO2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="AP2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="13">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1147,18 +1341,18 @@
       <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="8.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="8.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -1178,7 +1372,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1199,7 +1393,7 @@
         <v>No Team - Low Priority | 1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1220,7 +1414,7 @@
         <v>No Team - Medium Priority | 2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1241,7 +1435,7 @@
         <v>No Team - High Priority | 3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1262,7 +1456,7 @@
         <v>Farmer / Rep | 4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1283,7 +1477,7 @@
         <v>Giant's Keep | 5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1304,7 +1498,7 @@
         <v>Dragon's Lair | 6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1325,7 +1519,7 @@
         <v>Necropolis | 7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1346,7 +1540,7 @@
         <v>Steal Fortress | 8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1367,7 +1561,7 @@
         <v>Punisher's Crypt | 9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1388,7 +1582,7 @@
         <v>Hall of Magic | 10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1409,7 +1603,7 @@
         <v>Hall of Light | 11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1430,7 +1624,7 @@
         <v>Hall of Dark | 12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1451,7 +1645,7 @@
         <v>Hall of Fire | 13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1472,7 +1666,7 @@
         <v>Hall of Water | 14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1493,7 +1687,7 @@
         <v>Hall of Wind | 15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1514,7 +1708,7 @@
         <v>Hall of Heroes | 16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1535,7 +1729,7 @@
         <v>Trial of Ascension (Normal) | 17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1556,7 +1750,7 @@
         <v>Trial of Ascension (Hard) | 18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1577,7 +1771,7 @@
         <v>Trial of Ascension (Hell) | 19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1598,7 +1792,7 @@
         <v>Karzhan Remains - Griffon Lvl 4 (Dark) | 20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1619,7 +1813,7 @@
         <v>Karzhan Remains - Griffon Lvl 5 (Wind) | 21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1640,7 +1834,7 @@
         <v>Karzhan Remains - Inugami Lvl 4 (Light) | 22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1661,7 +1855,7 @@
         <v>Karzhan Remains - Inugami Lvl 5 (Dark) | 23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1682,7 +1876,7 @@
         <v>Karzhan Remains - Warbear Lvl 4 (Dark) | 24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1703,7 +1897,7 @@
         <v>Karzhan Remains - Warbear Lvl 5 (Fire) | 25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1724,7 +1918,7 @@
         <v>Ellunia Remains -  Fairy Lvl 4 (Wind) | 26</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1745,7 +1939,7 @@
         <v>Ellunia Remains -  Fairy Lvl 5 (Light) | 27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1766,7 +1960,7 @@
         <v>Ellunia Remains -  Pixie Lvl 4 (Wind) | 28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1787,7 +1981,7 @@
         <v>Ellunia Remains -  Pixie Lvl 5 (Water) | 29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1808,7 +2002,7 @@
         <v>Lumel Remains - Werewolf Lvl 4 (Light) | 30</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1829,7 +2023,7 @@
         <v>Lumel Remains - Werewolf Lvl 5 (Fire) | 31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1850,7 +2044,7 @@
         <v>Lumel Remains - Martial Cat Lvl 4 (Dark) | 32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1871,7 +2065,7 @@
         <v>Lumel Remains - Martial Cat Lvl 5 (Wind) | 33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1892,7 +2086,7 @@
         <v>Khalderun Remains - Howl Lvl 4 (Fire) | 34</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1913,7 +2107,7 @@
         <v>Khalderun Remains - Howl Lvl 5 (Water) | 35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1934,7 +2128,7 @@
         <v>Khalderun Remains - Grim Reaper Lvl 4 (Water) | 36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1955,7 +2149,7 @@
         <v>Khalderun Remains - Grim Reaper Lvl 5 (Dark) | 37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1976,7 +2170,7 @@
         <v>Karzhan - Forest of Roaring Beasts | 38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1997,7 +2191,7 @@
         <v>Ellunia - Sanctuary of Dreaming Fairies | 39</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2018,7 +2212,7 @@
         <v>Lumel - Cliff of Beast Men | 40</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2039,7 +2233,7 @@
         <v>Khalderun - Ruin of Silent Death | 41</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2060,7 +2254,7 @@
         <v>Dimension Hole Predator (Fire) | 42</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2081,7 +2275,7 @@
         <v>Dimension Hole Predator (Water) | 43</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2102,7 +2296,7 @@
         <v>Dimension Hole Predator (Wind) | 44</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2123,7 +2317,7 @@
         <v>Dimension Hole Predator (Light) | 45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2144,7 +2338,7 @@
         <v>Dimension Hole Predator (Dark) | 46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2165,7 +2359,7 @@
         <v>Rift of Worlds - Fire Beast | 47</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2186,7 +2380,7 @@
         <v>Rift of Worlds - Ice Beast | 48</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2207,7 +2401,7 @@
         <v>Rift of Worlds - Wind Beast | 49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2228,7 +2422,7 @@
         <v>Rift of Worlds - Light Beast | 50</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2249,7 +2443,7 @@
         <v>Rift of Worlds - Dark Beast | 51</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2270,7 +2464,7 @@
         <v>Rift Raid | 52</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2291,7 +2485,7 @@
         <v>Tartarus Labyrinth - Normal | 53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2312,7 +2506,7 @@
         <v>Tartarus Labyrinth - Rescue | 54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2333,7 +2527,7 @@
         <v>Tartarus Labyrinth - Explode | 55</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2354,7 +2548,7 @@
         <v>Tartarus Labyrinth - Cool Time | 56</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2375,7 +2569,7 @@
         <v>Tartarus Labyrinth - Speed Limit | 57</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2396,7 +2590,7 @@
         <v>Tartarus Labyrinth - Time Limit | 58</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2417,7 +2611,7 @@
         <v>Tartarus Labyrinth - Guilles | 59</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2438,7 +2632,7 @@
         <v>Tartarus Labyrinth - Kotos | 60</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2459,7 +2653,7 @@
         <v>Tartarus Labyrinth - Leos | 61</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2480,7 +2674,7 @@
         <v>Tartarus Labyrinth - Tartarus | 62</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2501,7 +2695,7 @@
         <v>Guild War Offense | 63</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2522,7 +2716,7 @@
         <v>Guild War Defense | 64</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2543,7 +2737,7 @@
         <v>Siege Battle Offense | 65</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2564,7 +2758,7 @@
         <v>Siege Battle Defense | 66</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2585,7 +2779,7 @@
         <v>Arena Offense | 67</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2606,7 +2800,7 @@
         <v>Arena Defense | 68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>

</xml_diff>